<commit_message>
Fixed Excel bugs who's depended on DrawBorders and FillReportDataFromModel functions
</commit_message>
<xml_diff>
--- a/Lection 3/task 3.1/ReportApp/Reports/Report.xlsx
+++ b/Lection 3/task 3.1/ReportApp/Reports/Report.xlsx
@@ -122,7 +122,7 @@
       <x:family val="2"/>
     </x:font>
   </x:fonts>
-  <x:fills count="3">
+  <x:fills count="5">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
@@ -135,8 +135,18 @@
         <x:bgColor indexed="64"/>
       </x:patternFill>
     </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFF5F5F5"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFFFFFFF"/>
+      </x:patternFill>
+    </x:fill>
   </x:fills>
-  <x:borders count="21">
+  <x:borders count="15">
     <x:border>
       <x:left/>
       <x:right/>
@@ -301,80 +311,12 @@
     </x:border>
     <x:border diagonalUp="0" diagonalDown="0">
       <x:left style="thin">
-        <x:color theme="0" tint="-0.499984740745262"/>
-      </x:left>
-      <x:right style="thin">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="thin">
-        <x:color theme="0" tint="-0.499984740745262"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
-    </x:border>
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
         <x:color rgb="FF000000"/>
       </x:left>
       <x:right style="thin">
         <x:color rgb="FF000000"/>
       </x:right>
       <x:top style="thin">
-        <x:color theme="0" tint="-0.499984740745262"/>
-      </x:top>
-      <x:bottom style="thin">
-        <x:color theme="0" tint="-0.499984740745262"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
-    </x:border>
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="thin">
-        <x:color indexed="64"/>
-      </x:left>
-      <x:right style="thin">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="thin">
-        <x:color theme="0" tint="-0.499984740745262"/>
-      </x:top>
-      <x:bottom style="thin">
-        <x:color indexed="64"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
-    </x:border>
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="thin">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
-    </x:border>
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="thin">
-        <x:color indexed="64"/>
-      </x:left>
-      <x:right style="thin">
-        <x:color indexed="64"/>
-      </x:right>
-      <x:top style="none">
         <x:color rgb="FF000000"/>
       </x:top>
       <x:bottom style="thin">
@@ -384,42 +326,8 @@
         <x:color rgb="FF000000"/>
       </x:diagonal>
     </x:border>
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="thin">
-        <x:color indexed="64"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="thin">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
-    </x:border>
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="thin">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="thin">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
-    </x:border>
   </x:borders>
-  <x:cellStyleXfs count="16">
+  <x:cellStyleXfs count="13">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -427,16 +335,13 @@
     <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="14" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="2" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="15" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="6" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="4" fillId="0" borderId="12" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -445,25 +350,19 @@
     <x:xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="16" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="17" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="20" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
@@ -523,10 +422,6 @@
       <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -535,27 +430,31 @@
       <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -909,16 +808,16 @@
       <x:c r="C7" s="19"/>
       <x:c r="D7" s="19"/>
       <x:c r="E7" s="19"/>
-      <x:c r="F7" s="20"/>
+      <x:c r="F7" s="19"/>
     </x:row>
     <x:row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <x:c r="B8" s="21" t="s">
+      <x:c r="B8" s="20" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="C8" s="22"/>
-      <x:c r="D8" s="22"/>
-      <x:c r="E8" s="22"/>
-      <x:c r="F8" s="23"/>
+      <x:c r="C8" s="21"/>
+      <x:c r="D8" s="21"/>
+      <x:c r="E8" s="21"/>
+      <x:c r="F8" s="22"/>
     </x:row>
     <x:row r="9" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <x:c r="B9" s="7" t="s">
@@ -933,21 +832,21 @@
       <x:c r="E9" s="8" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="F9" s="24" t="s">
+      <x:c r="F9" s="8" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <x:c r="B10" s="4" t="s">
+      <x:c r="B10" s="23" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="C10" s="2" t="s">
+      <x:c r="C10" s="24" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="D10" s="2" t="s">
+      <x:c r="D10" s="24" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="E10" s="2" t="s">
+      <x:c r="E10" s="24" t="s">
         <x:v>14</x:v>
       </x:c>
       <x:c r="F10" s="25" t="s">
@@ -958,16 +857,84 @@
       <x:c r="B11" s="26" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="C11" s="27" t="s">
+      <x:c r="C11" s="26" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="D11" s="27" t="s">
+      <x:c r="D11" s="26" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="E11" s="27" t="s">
+      <x:c r="E11" s="26" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="F11" s="28" t="s">
+      <x:c r="F11" s="27" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:9">
+      <x:c r="B12" s="28" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C12" s="28" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D12" s="28" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E12" s="28" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F12" s="28" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:9">
+      <x:c r="B13" s="27" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C13" s="27" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D13" s="27" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E13" s="27" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F13" s="27" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:9">
+      <x:c r="B14" s="28" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C14" s="28" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D14" s="28" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E14" s="28" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F14" s="28" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:9">
+      <x:c r="B15" s="27" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C15" s="27" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D15" s="27" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E15" s="27" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F15" s="27" t="s">
         <x:v>16</x:v>
       </x:c>
     </x:row>

</xml_diff>